<commit_message>
some more update for verification of fields on webpage.
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,18 +42,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +364,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refunction update in scripts.
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -15,9 +15,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>field3</t>
+  </si>
+  <si>
+    <t>field4</t>
+  </si>
+  <si>
+    <t>field5</t>
+  </si>
+  <si>
+    <t>field6</t>
+  </si>
+  <si>
+    <t>field7</t>
+  </si>
+  <si>
+    <t>field8</t>
+  </si>
+  <si>
+    <t>field9</t>
+  </si>
+  <si>
+    <t>Web1</t>
+  </si>
+  <si>
+    <t>Web2</t>
+  </si>
+  <si>
+    <t>Web3</t>
+  </si>
+  <si>
+    <t>Web4</t>
+  </si>
+  <si>
+    <t>Web5</t>
+  </si>
+  <si>
+    <t>Web6</t>
+  </si>
+  <si>
+    <t>Web7</t>
+  </si>
+  <si>
+    <t>Web8</t>
+  </si>
+  <si>
+    <t>Web9</t>
+  </si>
+  <si>
+    <t>row1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +90,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -61,9 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,74 +447,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>